<commit_message>
Elite Canada 2025 Synchro Added
</commit_message>
<xml_diff>
--- a/2025 World Games Ranking.xlsx
+++ b/2025 World Games Ranking.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorstirling/Library/CloudStorage/Dropbox/Documents/Trampoline/Websites/Trampoline Canada Website/Ranking Lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E030830-0E4C-7D49-92DB-E3157FED7F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AFE129-D9B5-C14D-AF66-FBCD2F361A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{A533BEEB-4696-DF41-A20A-D77C9379EBAE}"/>
   </bookViews>
   <sheets>
     <sheet name="DMT-W" sheetId="1" r:id="rId1"/>
     <sheet name="DMT-M" sheetId="2" r:id="rId2"/>
-    <sheet name="SYN-W" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="SYN-W" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DMT-M'!$A$1:$N$2</definedName>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
   <si>
     <t>Gabby Flynn</t>
   </si>
@@ -359,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,6 +382,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -423,13 +432,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -784,44 +793,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="20"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
@@ -858,34 +867,34 @@
       <c r="C3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="24">
-        <f>E3+F3</f>
+      <c r="D3" s="11">
+        <f t="shared" ref="D3:D20" si="0">E3+F3</f>
         <v>77.400000000000006</v>
       </c>
-      <c r="E3" s="24">
-        <f>MAX(G3+H3,K3+L3)</f>
+      <c r="E3" s="11">
+        <f t="shared" ref="E3:E20" si="1">MAX(G3+H3,K3+L3)</f>
         <v>51.8</v>
       </c>
-      <c r="F3" s="24">
-        <f>IF(G3+H3=K3+L3,MAX(G3,H3,I3,J3,K3,L3,M3,N3),IF(E3=G3+H3,MAX(I3,J3,K3,L3,M3,N3),MAX(G3,H3,I3,J3,M3,N3)))</f>
+      <c r="F3" s="11">
+        <f t="shared" ref="F3:F20" si="2">IF(G3+H3=K3+L3,MAX(G3,H3,I3,J3,K3,L3,M3,N3),IF(E3=G3+H3,MAX(I3,J3,K3,L3,M3,N3),MAX(G3,H3,I3,J3,M3,N3)))</f>
         <v>25.6</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="10">
         <v>25.7</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="11">
         <v>26.1</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="11">
         <v>25.6</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="12">
         <v>23.4</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="25"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" cm="1">
@@ -898,34 +907,34 @@
       <c r="C4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="24">
-        <f>E4+F4</f>
+      <c r="D4" s="11">
+        <f t="shared" si="0"/>
         <v>76.8</v>
       </c>
-      <c r="E4" s="24">
-        <f>MAX(G4+H4,K4+L4)</f>
+      <c r="E4" s="11">
+        <f t="shared" si="1"/>
         <v>51.099999999999994</v>
       </c>
-      <c r="F4" s="24">
-        <f>IF(G4+H4=K4+L4,MAX(G4,H4,I4,J4,K4,L4,M4,N4),IF(E4=G4+H4,MAX(I4,J4,K4,L4,M4,N4),MAX(G4,H4,I4,J4,M4,N4)))</f>
+      <c r="F4" s="11">
+        <f t="shared" si="2"/>
         <v>25.7</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="10">
         <v>25.9</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="11">
         <v>25.2</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="11">
         <v>25.7</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="12">
         <v>18.399999999999999</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="25"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="12"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" cm="1">
@@ -938,34 +947,34 @@
       <c r="C5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="24">
-        <f>E5+F5</f>
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
         <v>74.2</v>
       </c>
-      <c r="E5" s="24">
-        <f>MAX(G5+H5,K5+L5)</f>
+      <c r="E5" s="11">
+        <f t="shared" si="1"/>
         <v>48.7</v>
       </c>
-      <c r="F5" s="24">
-        <f>IF(G5+H5=K5+L5,MAX(G5,H5,I5,J5,K5,L5,M5,N5),IF(E5=G5+H5,MAX(I5,J5,K5,L5,M5,N5),MAX(G5,H5,I5,J5,M5,N5)))</f>
+      <c r="F5" s="11">
+        <f t="shared" si="2"/>
         <v>25.5</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="10">
         <v>24.5</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="11">
         <v>24.2</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="11">
         <v>25.5</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="12">
         <v>25</v>
       </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="25"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="12"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" cm="1">
@@ -978,34 +987,34 @@
       <c r="C6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="24">
-        <f>E6+F6</f>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
         <v>73.8</v>
       </c>
-      <c r="E6" s="24">
-        <f>MAX(G6+H6,K6+L6)</f>
+      <c r="E6" s="11">
+        <f t="shared" si="1"/>
         <v>49.1</v>
       </c>
-      <c r="F6" s="24">
-        <f>IF(G6+H6=K6+L6,MAX(G6,H6,I6,J6,K6,L6,M6,N6),IF(E6=G6+H6,MAX(I6,J6,K6,L6,M6,N6),MAX(G6,H6,I6,J6,M6,N6)))</f>
+      <c r="F6" s="11">
+        <f t="shared" si="2"/>
         <v>24.7</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="10">
         <v>23.5</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="11">
         <v>25.6</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="11">
         <v>24.7</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="12">
         <v>23.9</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="25"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" cm="1">
@@ -1018,34 +1027,34 @@
       <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="24">
-        <f>E7+F7</f>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
         <v>73.759999999999991</v>
       </c>
-      <c r="E7" s="24">
-        <f>MAX(G7+H7,K7+L7)</f>
+      <c r="E7" s="11">
+        <f t="shared" si="1"/>
         <v>48.26</v>
       </c>
-      <c r="F7" s="24">
-        <f>IF(G7+H7=K7+L7,MAX(G7,H7,I7,J7,K7,L7,M7,N7),IF(E7=G7+H7,MAX(I7,J7,K7,L7,M7,N7),MAX(G7,H7,I7,J7,M7,N7)))</f>
+      <c r="F7" s="11">
+        <f t="shared" si="2"/>
         <v>25.5</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="10">
         <v>25.06</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="11">
         <v>23.2</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="11">
         <v>25.5</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="12">
         <v>24.6</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="25"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" cm="1">
@@ -1058,34 +1067,34 @@
       <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="24">
-        <f>E8+F8</f>
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
         <v>72.699999999999989</v>
       </c>
-      <c r="E8" s="24">
-        <f>MAX(G8+H8,K8+L8)</f>
+      <c r="E8" s="11">
+        <f t="shared" si="1"/>
         <v>48.099999999999994</v>
       </c>
-      <c r="F8" s="24">
-        <f>IF(G8+H8=K8+L8,MAX(G8,H8,I8,J8,K8,L8,M8,N8),IF(E8=G8+H8,MAX(I8,J8,K8,L8,M8,N8),MAX(G8,H8,I8,J8,M8,N8)))</f>
+      <c r="F8" s="11">
+        <f t="shared" si="2"/>
         <v>24.6</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="10">
         <v>23.7</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="11">
         <v>24.4</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="11">
         <v>24.4</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="12">
         <v>24.6</v>
       </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="str" cm="1">
@@ -1096,34 +1105,34 @@
         <v>14</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="24">
-        <f>E9+F9</f>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
         <v>72.099999999999994</v>
       </c>
-      <c r="E9" s="24">
-        <f>MAX(G9+H9,K9+L9)</f>
+      <c r="E9" s="11">
+        <f t="shared" si="1"/>
         <v>48.9</v>
       </c>
-      <c r="F9" s="24">
-        <f>IF(G9+H9=K9+L9,MAX(G9,H9,I9,J9,K9,L9,M9,N9),IF(E9=G9+H9,MAX(I9,J9,K9,L9,M9,N9),MAX(G9,H9,I9,J9,M9,N9)))</f>
+      <c r="F9" s="11">
+        <f t="shared" si="2"/>
         <v>23.2</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="10">
         <v>24.2</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="11">
         <v>24.7</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="11">
         <v>23.2</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="12">
         <v>15</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="25"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" cm="1">
@@ -1136,34 +1145,34 @@
       <c r="C10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="24">
-        <f>E10+F10</f>
+      <c r="D10" s="11">
+        <f t="shared" si="0"/>
         <v>71.7</v>
       </c>
-      <c r="E10" s="24">
-        <f>MAX(G10+H10,K10+L10)</f>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
         <v>47.2</v>
       </c>
-      <c r="F10" s="24">
-        <f>IF(G10+H10=K10+L10,MAX(G10,H10,I10,J10,K10,L10,M10,N10),IF(E10=G10+H10,MAX(I10,J10,K10,L10,M10,N10),MAX(G10,H10,I10,J10,M10,N10)))</f>
+      <c r="F10" s="11">
+        <f t="shared" si="2"/>
         <v>24.5</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="10">
         <v>23.4</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="11">
         <v>23.8</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="11">
         <v>24.3</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="12">
         <v>24.5</v>
       </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="25"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="str" cm="1">
@@ -1174,34 +1183,34 @@
         <v>16</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="24">
-        <f>E11+F11</f>
+      <c r="D11" s="11">
+        <f t="shared" si="0"/>
         <v>69.099999999999994</v>
       </c>
-      <c r="E11" s="24">
-        <f>MAX(G11+H11,K11+L11)</f>
+      <c r="E11" s="11">
+        <f t="shared" si="1"/>
         <v>48.5</v>
       </c>
-      <c r="F11" s="24">
-        <f>IF(G11+H11=K11+L11,MAX(G11,H11,I11,J11,K11,L11,M11,N11),IF(E11=G11+H11,MAX(I11,J11,K11,L11,M11,N11),MAX(G11,H11,I11,J11,M11,N11)))</f>
+      <c r="F11" s="11">
+        <f t="shared" si="2"/>
         <v>20.6</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="10">
         <v>24.4</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="11">
         <v>24.1</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="11">
         <v>20.6</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="12">
         <v>17.8</v>
       </c>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="25"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="str" cm="1">
@@ -1212,34 +1221,34 @@
         <v>12</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="24">
-        <f>E12+F12</f>
+      <c r="D12" s="11">
+        <f t="shared" si="0"/>
         <v>67.2</v>
       </c>
-      <c r="E12" s="24">
-        <f>MAX(G12+H12,K12+L12)</f>
+      <c r="E12" s="11">
+        <f t="shared" si="1"/>
         <v>49.4</v>
       </c>
-      <c r="F12" s="24">
-        <f>IF(G12+H12=K12+L12,MAX(G12,H12,I12,J12,K12,L12,M12,N12),IF(E12=G12+H12,MAX(I12,J12,K12,L12,M12,N12),MAX(G12,H12,I12,J12,M12,N12)))</f>
+      <c r="F12" s="11">
+        <f t="shared" si="2"/>
         <v>17.8</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="10">
         <v>25</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="11">
         <v>24.4</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="11">
         <v>17.8</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="12">
         <v>17.5</v>
       </c>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="str" cm="1">
@@ -1250,30 +1259,30 @@
         <v>20</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="24">
-        <f>E13+F13</f>
+      <c r="D13" s="11">
+        <f t="shared" si="0"/>
         <v>47.2</v>
       </c>
-      <c r="E13" s="24">
-        <f>MAX(G13+H13,K13+L13)</f>
+      <c r="E13" s="11">
+        <f t="shared" si="1"/>
         <v>47.2</v>
       </c>
-      <c r="F13" s="24">
-        <f>IF(G13+H13=K13+L13,MAX(G13,H13,I13,J13,K13,L13,M13,N13),IF(E13=G13+H13,MAX(I13,J13,K13,L13,M13,N13),MAX(G13,H13,I13,J13,M13,N13)))</f>
+      <c r="F13" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="10">
         <v>23.8</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="11">
         <v>23.4</v>
       </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="str" cm="1">
@@ -1284,30 +1293,30 @@
         <v>21</v>
       </c>
       <c r="C14" s="9"/>
-      <c r="D14" s="24">
-        <f>E14+F14</f>
+      <c r="D14" s="11">
+        <f t="shared" si="0"/>
         <v>46.4</v>
       </c>
-      <c r="E14" s="24">
-        <f>MAX(G14+H14,K14+L14)</f>
+      <c r="E14" s="11">
+        <f t="shared" si="1"/>
         <v>46.4</v>
       </c>
-      <c r="F14" s="24">
-        <f>IF(G14+H14=K14+L14,MAX(G14,H14,I14,J14,K14,L14,M14,N14),IF(E14=G14+H14,MAX(I14,J14,K14,L14,M14,N14),MAX(G14,H14,I14,J14,M14,N14)))</f>
+      <c r="F14" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="10">
         <v>22.2</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="11">
         <v>24.2</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="12"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="str" cm="1">
@@ -1318,30 +1327,30 @@
         <v>22</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="24">
-        <f>E15+F15</f>
+      <c r="D15" s="11">
+        <f t="shared" si="0"/>
         <v>41.5</v>
       </c>
-      <c r="E15" s="24">
-        <f>MAX(G15+H15,K15+L15)</f>
+      <c r="E15" s="11">
+        <f t="shared" si="1"/>
         <v>41.5</v>
       </c>
-      <c r="F15" s="24">
-        <f>IF(G15+H15=K15+L15,MAX(G15,H15,I15,J15,K15,L15,M15,N15),IF(E15=G15+H15,MAX(I15,J15,K15,L15,M15,N15),MAX(G15,H15,I15,J15,M15,N15)))</f>
+      <c r="F15" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="10">
         <v>17.8</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="11">
         <v>23.7</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="25"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="str" cm="1">
@@ -1352,30 +1361,30 @@
         <v>23</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="24">
-        <f>E16+F16</f>
+      <c r="D16" s="11">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="E16" s="24">
-        <f>MAX(G16+H16,K16+L16)</f>
+      <c r="E16" s="11">
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="F16" s="24">
-        <f>IF(G16+H16=K16+L16,MAX(G16,H16,I16,J16,K16,L16,M16,N16),IF(E16=G16+H16,MAX(I16,J16,K16,L16,M16,N16),MAX(G16,H16,I16,J16,M16,N16)))</f>
+      <c r="F16" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="10">
         <v>17.600000000000001</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="11">
         <v>23.4</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="25"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="12"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="str" cm="1">
@@ -1386,30 +1395,30 @@
         <v>24</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="24">
-        <f>E17+F17</f>
+      <c r="D17" s="11">
+        <f t="shared" si="0"/>
         <v>39.099999999999994</v>
       </c>
-      <c r="E17" s="24">
-        <f>MAX(G17+H17,K17+L17)</f>
+      <c r="E17" s="11">
+        <f t="shared" si="1"/>
         <v>39.099999999999994</v>
       </c>
-      <c r="F17" s="24">
-        <f>IF(G17+H17=K17+L17,MAX(G17,H17,I17,J17,K17,L17,M17,N17),IF(E17=G17+H17,MAX(I17,J17,K17,L17,M17,N17),MAX(G17,H17,I17,J17,M17,N17)))</f>
+      <c r="F17" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="10">
         <v>23.9</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="11">
         <v>15.2</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="25"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="12"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="str" cm="1">
@@ -1420,30 +1429,30 @@
         <v>25</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="24">
-        <f>E18+F18</f>
+      <c r="D18" s="11">
+        <f t="shared" si="0"/>
         <v>32.799999999999997</v>
       </c>
-      <c r="E18" s="24">
-        <f>MAX(G18+H18,K18+L18)</f>
+      <c r="E18" s="11">
+        <f t="shared" si="1"/>
         <v>32.799999999999997</v>
       </c>
-      <c r="F18" s="24">
-        <f>IF(G18+H18=K18+L18,MAX(G18,H18,I18,J18,K18,L18,M18,N18),IF(E18=G18+H18,MAX(I18,J18,K18,L18,M18,N18),MAX(G18,H18,I18,J18,M18,N18)))</f>
+      <c r="F18" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="10">
         <v>17.600000000000001</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="11">
         <v>15.2</v>
       </c>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="str" cm="1">
@@ -1454,30 +1463,30 @@
         <v>26</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="24">
-        <f>E19+F19</f>
+      <c r="D19" s="11">
+        <f t="shared" si="0"/>
         <v>24.5</v>
       </c>
-      <c r="E19" s="24">
-        <f>MAX(G19+H19,K19+L19)</f>
+      <c r="E19" s="11">
+        <f t="shared" si="1"/>
         <v>24.5</v>
       </c>
-      <c r="F19" s="24">
-        <f>IF(G19+H19=K19+L19,MAX(G19,H19,I19,J19,K19,L19,M19,N19),IF(E19=G19+H19,MAX(I19,J19,K19,L19,M19,N19),MAX(G19,H19,I19,J19,M19,N19)))</f>
+      <c r="F19" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="10">
         <v>0</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="11">
         <v>24.5</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="25"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="12"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="str" cm="1">
@@ -1488,30 +1497,30 @@
         <v>27</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="24">
-        <f>E20+F20</f>
+      <c r="D20" s="11">
+        <f t="shared" si="0"/>
         <v>20.5</v>
       </c>
-      <c r="E20" s="24">
-        <f>MAX(G20+H20,K20+L20)</f>
+      <c r="E20" s="11">
+        <f t="shared" si="1"/>
         <v>20.5</v>
       </c>
-      <c r="F20" s="24">
-        <f>IF(G20+H20=K20+L20,MAX(G20,H20,I20,J20,K20,L20,M20,N20),IF(E20=G20+H20,MAX(I20,J20,K20,L20,M20,N20),MAX(G20,H20,I20,J20,M20,N20)))</f>
+      <c r="F20" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="10">
         <v>20.5</v>
       </c>
-      <c r="H20" s="24">
+      <c r="H20" s="11">
         <v>0</v>
       </c>
-      <c r="I20" s="24"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="12"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="str" cm="1">
@@ -2999,44 +3008,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="20"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
@@ -3073,34 +3082,34 @@
       <c r="C3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="24">
-        <f>E3+F3</f>
+      <c r="D3" s="11">
+        <f t="shared" ref="D3:D28" si="0">E3+F3</f>
         <v>81.2</v>
       </c>
-      <c r="E3" s="24">
-        <f>MAX(G3+H3,K3+L3)</f>
+      <c r="E3" s="11">
+        <f t="shared" ref="E3:E28" si="1">MAX(G3+H3,K3+L3)</f>
         <v>53.6</v>
       </c>
-      <c r="F3" s="24">
-        <f>IF(G3+H3=K3+L3,MAX(G3,H3,I3,J3,K3,L3,M3,N3),IF(E3=G3+H3,MAX(I3,J3,K3,L3,M3,N3),MAX(G3,H3,I3,J3,M3,N3)))</f>
+      <c r="F3" s="11">
+        <f t="shared" ref="F3:F28" si="2">IF(G3+H3=K3+L3,MAX(G3,H3,I3,J3,K3,L3,M3,N3),IF(E3=G3+H3,MAX(I3,J3,K3,L3,M3,N3),MAX(G3,H3,I3,J3,M3,N3)))</f>
         <v>27.6</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="10">
         <v>27.3</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="11">
         <v>26.3</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="11">
         <v>27.6</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="12">
         <v>27.3</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="25"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" cm="1">
@@ -3113,34 +3122,34 @@
       <c r="C4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="24">
-        <f>E4+F4</f>
+      <c r="D4" s="11">
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="E4" s="24">
-        <f>MAX(G4+H4,K4+L4)</f>
+      <c r="E4" s="11">
+        <f t="shared" si="1"/>
         <v>54.2</v>
       </c>
-      <c r="F4" s="24">
-        <f>IF(G4+H4=K4+L4,MAX(G4,H4,I4,J4,K4,L4,M4,N4),IF(E4=G4+H4,MAX(I4,J4,K4,L4,M4,N4),MAX(G4,H4,I4,J4,M4,N4)))</f>
+      <c r="F4" s="11">
+        <f t="shared" si="2"/>
         <v>26.8</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="10">
         <v>27.4</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="11">
         <v>26.8</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="11">
         <v>26.8</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="12">
         <v>25.7</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="25"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="12"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" cm="1">
@@ -3153,34 +3162,34 @@
       <c r="C5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="24">
-        <f>E5+F5</f>
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
         <v>80.2</v>
       </c>
-      <c r="E5" s="24">
-        <f>MAX(G5+H5,K5+L5)</f>
+      <c r="E5" s="11">
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="F5" s="24">
-        <f>IF(G5+H5=K5+L5,MAX(G5,H5,I5,J5,K5,L5,M5,N5),IF(E5=G5+H5,MAX(I5,J5,K5,L5,M5,N5),MAX(G5,H5,I5,J5,M5,N5)))</f>
+      <c r="F5" s="11">
+        <f t="shared" si="2"/>
         <v>27.2</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="10">
         <v>27</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="11">
         <v>26</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="11">
         <v>23.3</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="12">
         <v>27.2</v>
       </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="25"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="12"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" cm="1">
@@ -3193,34 +3202,34 @@
       <c r="C6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="24">
-        <f>E6+F6</f>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
         <v>79.900000000000006</v>
       </c>
-      <c r="E6" s="24">
-        <f>MAX(G6+H6,K6+L6)</f>
+      <c r="E6" s="11">
+        <f t="shared" si="1"/>
         <v>52.6</v>
       </c>
-      <c r="F6" s="24">
-        <f>IF(G6+H6=K6+L6,MAX(G6,H6,I6,J6,K6,L6,M6,N6),IF(E6=G6+H6,MAX(I6,J6,K6,L6,M6,N6),MAX(G6,H6,I6,J6,M6,N6)))</f>
+      <c r="F6" s="11">
+        <f t="shared" si="2"/>
         <v>27.3</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="10">
         <v>26.1</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="11">
         <v>26.5</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="11">
         <v>26.7</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="12">
         <v>27.3</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="25"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" cm="1">
@@ -3233,34 +3242,34 @@
       <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="24">
-        <f>E7+F7</f>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
         <v>79.099999999999994</v>
       </c>
-      <c r="E7" s="24">
-        <f>MAX(G7+H7,K7+L7)</f>
+      <c r="E7" s="11">
+        <f t="shared" si="1"/>
         <v>52.7</v>
       </c>
-      <c r="F7" s="24">
-        <f>IF(G7+H7=K7+L7,MAX(G7,H7,I7,J7,K7,L7,M7,N7),IF(E7=G7+H7,MAX(I7,J7,K7,L7,M7,N7),MAX(G7,H7,I7,J7,M7,N7)))</f>
+      <c r="F7" s="11">
+        <f t="shared" si="2"/>
         <v>26.4</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="10">
         <v>27</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="11">
         <v>25.7</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="11">
         <v>26.4</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="12">
         <v>25.7</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="25"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="str" cm="1">
@@ -3271,34 +3280,34 @@
         <v>36</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="24">
-        <f>E8+F8</f>
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
         <v>77.7</v>
       </c>
-      <c r="E8" s="24">
-        <f>MAX(G8+H8,K8+L8)</f>
+      <c r="E8" s="11">
+        <f t="shared" si="1"/>
         <v>51.1</v>
       </c>
-      <c r="F8" s="24">
-        <f>IF(G8+H8=K8+L8,MAX(G8,H8,I8,J8,K8,L8,M8,N8),IF(E8=G8+H8,MAX(I8,J8,K8,L8,M8,N8),MAX(G8,H8,I8,J8,M8,N8)))</f>
+      <c r="F8" s="11">
+        <f t="shared" si="2"/>
         <v>26.6</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="10">
         <v>26.1</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="11">
         <v>25</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="11">
         <v>20.5</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="12">
         <v>26.6</v>
       </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="str" cm="1">
@@ -3309,34 +3318,34 @@
         <v>38</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="24">
-        <f>E9+F9</f>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
         <v>76.5</v>
       </c>
-      <c r="E9" s="24">
-        <f>MAX(G9+H9,K9+L9)</f>
+      <c r="E9" s="11">
+        <f t="shared" si="1"/>
         <v>50.1</v>
       </c>
-      <c r="F9" s="24">
-        <f>IF(G9+H9=K9+L9,MAX(G9,H9,I9,J9,K9,L9,M9,N9),IF(E9=G9+H9,MAX(I9,J9,K9,L9,M9,N9),MAX(G9,H9,I9,J9,M9,N9)))</f>
+      <c r="F9" s="11">
+        <f t="shared" si="2"/>
         <v>26.4</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="10">
         <v>25</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="11">
         <v>25.1</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="11">
         <v>26.4</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="12">
         <v>24.1</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="25"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="str" cm="1">
@@ -3347,34 +3356,34 @@
         <v>37</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="24">
-        <f>E10+F10</f>
+      <c r="D10" s="11">
+        <f t="shared" si="0"/>
         <v>75.7</v>
       </c>
-      <c r="E10" s="24">
-        <f>MAX(G10+H10,K10+L10)</f>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
         <v>50.9</v>
       </c>
-      <c r="F10" s="24">
-        <f>IF(G10+H10=K10+L10,MAX(G10,H10,I10,J10,K10,L10,M10,N10),IF(E10=G10+H10,MAX(I10,J10,K10,L10,M10,N10),MAX(G10,H10,I10,J10,M10,N10)))</f>
+      <c r="F10" s="11">
+        <f t="shared" si="2"/>
         <v>24.8</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="10">
         <v>26.2</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="11">
         <v>24.7</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="11">
         <v>24.7</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="12">
         <v>24.8</v>
       </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="25"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="str" cm="1">
@@ -3385,34 +3394,34 @@
         <v>39</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="24">
-        <f>E11+F11</f>
+      <c r="D11" s="11">
+        <f t="shared" si="0"/>
         <v>75.400000000000006</v>
       </c>
-      <c r="E11" s="24">
-        <f>MAX(G11+H11,K11+L11)</f>
+      <c r="E11" s="11">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="F11" s="24">
-        <f>IF(G11+H11=K11+L11,MAX(G11,H11,I11,J11,K11,L11,M11,N11),IF(E11=G11+H11,MAX(I11,J11,K11,L11,M11,N11),MAX(G11,H11,I11,J11,M11,N11)))</f>
+      <c r="F11" s="11">
+        <f t="shared" si="2"/>
         <v>25.4</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="10">
         <v>24.9</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="11">
         <v>25.1</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="11">
         <v>25.4</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="12">
         <v>25.4</v>
       </c>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="25"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="str" cm="1">
@@ -3423,34 +3432,34 @@
         <v>40</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="24">
-        <f>E12+F12</f>
+      <c r="D12" s="11">
+        <f t="shared" si="0"/>
         <v>75.099999999999994</v>
       </c>
-      <c r="E12" s="24">
-        <f>MAX(G12+H12,K12+L12)</f>
+      <c r="E12" s="11">
+        <f t="shared" si="1"/>
         <v>49.2</v>
       </c>
-      <c r="F12" s="24">
-        <f>IF(G12+H12=K12+L12,MAX(G12,H12,I12,J12,K12,L12,M12,N12),IF(E12=G12+H12,MAX(I12,J12,K12,L12,M12,N12),MAX(G12,H12,I12,J12,M12,N12)))</f>
+      <c r="F12" s="11">
+        <f t="shared" si="2"/>
         <v>25.9</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="10">
         <v>24.6</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="11">
         <v>24.6</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="11">
         <v>25.9</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="12">
         <v>24.2</v>
       </c>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="str" cm="1">
@@ -3461,30 +3470,30 @@
         <v>41</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="24">
-        <f>E13+F13</f>
+      <c r="D13" s="11">
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="E13" s="24">
-        <f>MAX(G13+H13,K13+L13)</f>
+      <c r="E13" s="11">
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="F13" s="24">
-        <f>IF(G13+H13=K13+L13,MAX(G13,H13,I13,J13,K13,L13,M13,N13),IF(E13=G13+H13,MAX(I13,J13,K13,L13,M13,N13),MAX(G13,H13,I13,J13,M13,N13)))</f>
+      <c r="F13" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="10">
         <v>23.2</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="11">
         <v>25.8</v>
       </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" cm="1">
@@ -3497,30 +3506,30 @@
       <c r="C14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="24">
-        <f>E14+F14</f>
+      <c r="D14" s="11">
+        <f t="shared" si="0"/>
         <v>48.2</v>
       </c>
-      <c r="E14" s="24">
-        <f>MAX(G14+H14,K14+L14)</f>
+      <c r="E14" s="11">
+        <f t="shared" si="1"/>
         <v>48.2</v>
       </c>
-      <c r="F14" s="24">
-        <f>IF(G14+H14=K14+L14,MAX(G14,H14,I14,J14,K14,L14,M14,N14),IF(E14=G14+H14,MAX(I14,J14,K14,L14,M14,N14),MAX(G14,H14,I14,J14,M14,N14)))</f>
+      <c r="F14" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="10">
         <v>19.3</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="11">
         <v>28.9</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="12"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="str" cm="1">
@@ -3531,30 +3540,30 @@
         <v>43</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="24">
-        <f>E15+F15</f>
+      <c r="D15" s="11">
+        <f t="shared" si="0"/>
         <v>48.1</v>
       </c>
-      <c r="E15" s="24">
-        <f>MAX(G15+H15,K15+L15)</f>
+      <c r="E15" s="11">
+        <f t="shared" si="1"/>
         <v>48.1</v>
       </c>
-      <c r="F15" s="24">
-        <f>IF(G15+H15=K15+L15,MAX(G15,H15,I15,J15,K15,L15,M15,N15),IF(E15=G15+H15,MAX(I15,J15,K15,L15,M15,N15),MAX(G15,H15,I15,J15,M15,N15)))</f>
+      <c r="F15" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="10">
         <v>24.6</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="11">
         <v>23.5</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="25"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="str" cm="1">
@@ -3565,30 +3574,30 @@
         <v>44</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="24">
-        <f>E16+F16</f>
+      <c r="D16" s="11">
+        <f t="shared" si="0"/>
         <v>46.8</v>
       </c>
-      <c r="E16" s="24">
-        <f>MAX(G16+H16,K16+L16)</f>
+      <c r="E16" s="11">
+        <f t="shared" si="1"/>
         <v>46.8</v>
       </c>
-      <c r="F16" s="24">
-        <f>IF(G16+H16=K16+L16,MAX(G16,H16,I16,J16,K16,L16,M16,N16),IF(E16=G16+H16,MAX(I16,J16,K16,L16,M16,N16),MAX(G16,H16,I16,J16,M16,N16)))</f>
+      <c r="F16" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="10">
         <v>21.7</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="11">
         <v>25.1</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="25"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="12"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="str" cm="1">
@@ -3599,30 +3608,30 @@
         <v>45</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="24">
-        <f>E17+F17</f>
+      <c r="D17" s="11">
+        <f t="shared" si="0"/>
         <v>46.7</v>
       </c>
-      <c r="E17" s="24">
-        <f>MAX(G17+H17,K17+L17)</f>
+      <c r="E17" s="11">
+        <f t="shared" si="1"/>
         <v>46.7</v>
       </c>
-      <c r="F17" s="24">
-        <f>IF(G17+H17=K17+L17,MAX(G17,H17,I17,J17,K17,L17,M17,N17),IF(E17=G17+H17,MAX(I17,J17,K17,L17,M17,N17),MAX(G17,H17,I17,J17,M17,N17)))</f>
+      <c r="F17" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="10">
         <v>24.7</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="11">
         <v>22</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="25"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="12"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="str" cm="1">
@@ -3633,30 +3642,30 @@
         <v>46</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="24">
-        <f>E18+F18</f>
+      <c r="D18" s="11">
+        <f t="shared" si="0"/>
         <v>46.7</v>
       </c>
-      <c r="E18" s="24">
-        <f>MAX(G18+H18,K18+L18)</f>
+      <c r="E18" s="11">
+        <f t="shared" si="1"/>
         <v>46.7</v>
       </c>
-      <c r="F18" s="24">
-        <f>IF(G18+H18=K18+L18,MAX(G18,H18,I18,J18,K18,L18,M18,N18),IF(E18=G18+H18,MAX(I18,J18,K18,L18,M18,N18),MAX(G18,H18,I18,J18,M18,N18)))</f>
+      <c r="F18" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="10">
         <v>25.2</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="11">
         <v>21.5</v>
       </c>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="str" cm="1">
@@ -3667,30 +3676,30 @@
         <v>47</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="24">
-        <f>E19+F19</f>
+      <c r="D19" s="11">
+        <f t="shared" si="0"/>
         <v>46.5</v>
       </c>
-      <c r="E19" s="24">
-        <f>MAX(G19+H19,K19+L19)</f>
+      <c r="E19" s="11">
+        <f t="shared" si="1"/>
         <v>46.5</v>
       </c>
-      <c r="F19" s="24">
-        <f>IF(G19+H19=K19+L19,MAX(G19,H19,I19,J19,K19,L19,M19,N19),IF(E19=G19+H19,MAX(I19,J19,K19,L19,M19,N19),MAX(G19,H19,I19,J19,M19,N19)))</f>
+      <c r="F19" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="10">
         <v>22.9</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="11">
         <v>23.6</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="25"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="12"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="str" cm="1">
@@ -3701,30 +3710,30 @@
         <v>48</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="24">
-        <f>E20+F20</f>
+      <c r="D20" s="11">
+        <f t="shared" si="0"/>
         <v>46.4</v>
       </c>
-      <c r="E20" s="24">
-        <f>MAX(G20+H20,K20+L20)</f>
+      <c r="E20" s="11">
+        <f t="shared" si="1"/>
         <v>46.4</v>
       </c>
-      <c r="F20" s="24">
-        <f>IF(G20+H20=K20+L20,MAX(G20,H20,I20,J20,K20,L20,M20,N20),IF(E20=G20+H20,MAX(I20,J20,K20,L20,M20,N20),MAX(G20,H20,I20,J20,M20,N20)))</f>
+      <c r="F20" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="10">
         <v>26</v>
       </c>
-      <c r="H20" s="24">
+      <c r="H20" s="11">
         <v>20.399999999999999</v>
       </c>
-      <c r="I20" s="24"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="12"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="str" cm="1">
@@ -3735,30 +3744,30 @@
         <v>49</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="24">
-        <f>E21+F21</f>
+      <c r="D21" s="11">
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
-      <c r="E21" s="24">
-        <f>MAX(G21+H21,K21+L21)</f>
+      <c r="E21" s="11">
+        <f t="shared" si="1"/>
         <v>46.2</v>
       </c>
-      <c r="F21" s="24">
-        <f>IF(G21+H21=K21+L21,MAX(G21,H21,I21,J21,K21,L21,M21,N21),IF(E21=G21+H21,MAX(I21,J21,K21,L21,M21,N21),MAX(G21,H21,I21,J21,M21,N21)))</f>
+      <c r="F21" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="10">
         <v>24</v>
       </c>
-      <c r="H21" s="24">
+      <c r="H21" s="11">
         <v>22.2</v>
       </c>
-      <c r="I21" s="24"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="25"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="12"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="str" cm="1">
@@ -3769,30 +3778,30 @@
         <v>50</v>
       </c>
       <c r="C22" s="9"/>
-      <c r="D22" s="24">
-        <f>E22+F22</f>
+      <c r="D22" s="11">
+        <f t="shared" si="0"/>
         <v>44.3</v>
       </c>
-      <c r="E22" s="24">
-        <f>MAX(G22+H22,K22+L22)</f>
+      <c r="E22" s="11">
+        <f t="shared" si="1"/>
         <v>44.3</v>
       </c>
-      <c r="F22" s="24">
-        <f>IF(G22+H22=K22+L22,MAX(G22,H22,I22,J22,K22,L22,M22,N22),IF(E22=G22+H22,MAX(I22,J22,K22,L22,M22,N22),MAX(G22,H22,I22,J22,M22,N22)))</f>
+      <c r="F22" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="10">
         <v>25.9</v>
       </c>
-      <c r="H22" s="24">
+      <c r="H22" s="11">
         <v>18.399999999999999</v>
       </c>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="25"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="12"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="str" cm="1">
@@ -3803,30 +3812,30 @@
         <v>51</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="24">
-        <f>E23+F23</f>
+      <c r="D23" s="11">
+        <f t="shared" si="0"/>
         <v>43.4</v>
       </c>
-      <c r="E23" s="24">
-        <f>MAX(G23+H23,K23+L23)</f>
+      <c r="E23" s="11">
+        <f t="shared" si="1"/>
         <v>43.4</v>
       </c>
-      <c r="F23" s="24">
-        <f>IF(G23+H23=K23+L23,MAX(G23,H23,I23,J23,K23,L23,M23,N23),IF(E23=G23+H23,MAX(I23,J23,K23,L23,M23,N23),MAX(G23,H23,I23,J23,M23,N23)))</f>
+      <c r="F23" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="10">
         <v>18.2</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H23" s="11">
         <v>25.2</v>
       </c>
-      <c r="I23" s="24"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="25"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="12"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="str" cm="1">
@@ -3837,30 +3846,30 @@
         <v>52</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="24">
-        <f>E24+F24</f>
+      <c r="D24" s="11">
+        <f t="shared" si="0"/>
         <v>41.5</v>
       </c>
-      <c r="E24" s="24">
-        <f>MAX(G24+H24,K24+L24)</f>
+      <c r="E24" s="11">
+        <f t="shared" si="1"/>
         <v>41.5</v>
       </c>
-      <c r="F24" s="24">
-        <f>IF(G24+H24=K24+L24,MAX(G24,H24,I24,J24,K24,L24,M24,N24),IF(E24=G24+H24,MAX(I24,J24,K24,L24,M24,N24),MAX(G24,H24,I24,J24,M24,N24)))</f>
+      <c r="F24" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="10">
         <v>21.2</v>
       </c>
-      <c r="H24" s="24">
+      <c r="H24" s="11">
         <v>20.3</v>
       </c>
-      <c r="I24" s="24"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="25"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" cm="1">
@@ -3873,30 +3882,30 @@
       <c r="C25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="24">
-        <f>E25+F25</f>
+      <c r="D25" s="11">
+        <f t="shared" si="0"/>
         <v>29.6</v>
       </c>
-      <c r="E25" s="24">
-        <f>MAX(G25+H25,K25+L25)</f>
+      <c r="E25" s="11">
+        <f t="shared" si="1"/>
         <v>29.6</v>
       </c>
-      <c r="F25" s="24">
-        <f>IF(G25+H25=K25+L25,MAX(G25,H25,I25,J25,K25,L25,M25,N25),IF(E25=G25+H25,MAX(I25,J25,K25,L25,M25,N25),MAX(G25,H25,I25,J25,M25,N25)))</f>
+      <c r="F25" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G25" s="23">
+      <c r="G25" s="10">
         <v>29.6</v>
       </c>
-      <c r="H25" s="24">
+      <c r="H25" s="11">
         <v>0</v>
       </c>
-      <c r="I25" s="24"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="25"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="12"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="str" cm="1">
@@ -3907,30 +3916,30 @@
         <v>54</v>
       </c>
       <c r="C26" s="9"/>
-      <c r="D26" s="24">
-        <f>E26+F26</f>
+      <c r="D26" s="11">
+        <f t="shared" si="0"/>
         <v>26.1</v>
       </c>
-      <c r="E26" s="24">
-        <f>MAX(G26+H26,K26+L26)</f>
+      <c r="E26" s="11">
+        <f t="shared" si="1"/>
         <v>26.1</v>
       </c>
-      <c r="F26" s="24">
-        <f>IF(G26+H26=K26+L26,MAX(G26,H26,I26,J26,K26,L26,M26,N26),IF(E26=G26+H26,MAX(I26,J26,K26,L26,M26,N26),MAX(G26,H26,I26,J26,M26,N26)))</f>
+      <c r="F26" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="10">
         <v>0</v>
       </c>
-      <c r="H26" s="24">
+      <c r="H26" s="11">
         <v>26.1</v>
       </c>
-      <c r="I26" s="24"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="25"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" cm="1">
@@ -3943,30 +3952,30 @@
       <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="24">
-        <f>E27+F27</f>
+      <c r="D27" s="11">
+        <f t="shared" si="0"/>
         <v>24.1</v>
       </c>
-      <c r="E27" s="24">
-        <f>MAX(G27+H27,K27+L27)</f>
+      <c r="E27" s="11">
+        <f t="shared" si="1"/>
         <v>24.1</v>
       </c>
-      <c r="F27" s="24">
-        <f>IF(G27+H27=K27+L27,MAX(G27,H27,I27,J27,K27,L27,M27,N27),IF(E27=G27+H27,MAX(I27,J27,K27,L27,M27,N27),MAX(G27,H27,I27,J27,M27,N27)))</f>
+      <c r="F27" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27" s="10">
         <v>24.1</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="11">
         <v>0</v>
       </c>
-      <c r="I27" s="24"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="25"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="12"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="str" cm="1">
@@ -3977,30 +3986,30 @@
         <v>56</v>
       </c>
       <c r="C28" s="9"/>
-      <c r="D28" s="24">
-        <f>E28+F28</f>
+      <c r="D28" s="11">
+        <f t="shared" si="0"/>
         <v>22.8</v>
       </c>
-      <c r="E28" s="24">
-        <f>MAX(G28+H28,K28+L28)</f>
+      <c r="E28" s="11">
+        <f t="shared" si="1"/>
         <v>22.8</v>
       </c>
-      <c r="F28" s="24">
-        <f>IF(G28+H28=K28+L28,MAX(G28,H28,I28,J28,K28,L28,M28,N28),IF(E28=G28+H28,MAX(I28,J28,K28,L28,M28,N28),MAX(G28,H28,I28,J28,M28,N28)))</f>
+      <c r="F28" s="11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="10">
         <v>22.8</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="11">
         <v>0</v>
       </c>
-      <c r="I28" s="24"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="25"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="str" cm="1">
@@ -5343,42 +5352,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="14" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="16"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="7" t="s">
         <v>62</v>
       </c>
@@ -5409,57 +5418,71 @@
       <c r="C3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="26">
         <f>E3+F3</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="24">
+        <v>97.94</v>
+      </c>
+      <c r="E3" s="26">
         <f>MAX(G3:L3)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="24">
+        <v>49.13</v>
+      </c>
+      <c r="F3" s="26">
         <f>IF(COUNT(G3:L3)&gt;1,LARGE(G3:L3,2),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="3"/>
+        <v>48.81</v>
+      </c>
+      <c r="G3" s="27">
+        <v>48.81</v>
+      </c>
+      <c r="H3" s="26">
+        <v>49.13</v>
+      </c>
+      <c r="I3" s="26">
+        <v>9.69</v>
+      </c>
+      <c r="J3" s="27"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="28"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="str" cm="1">
+      <c r="A4" cm="1">
         <f t="array" ref="A4">IF(C4="P",SUMPRODUCT(--(D$3:D$100&gt;D4),--(C$3:C$100="P"))+1,"")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="24">
+      <c r="C4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="26">
         <f>E4+F4</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="24">
-        <f t="shared" ref="E4:E7" si="0">MAX(G4:L4)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="24">
-        <f t="shared" ref="F4:F7" si="1">IF(COUNT(G4:L4)&gt;1,LARGE(G4:L4,2),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="3"/>
+        <v>94.830000000000013</v>
+      </c>
+      <c r="E4" s="26">
+        <f>MAX(G4:L4)</f>
+        <v>47.7</v>
+      </c>
+      <c r="F4" s="26">
+        <f>IF(COUNT(G4:L4)&gt;1,LARGE(G4:L4,2),0)</f>
+        <v>47.13</v>
+      </c>
+      <c r="G4" s="27">
+        <v>47.7</v>
+      </c>
+      <c r="H4" s="26">
+        <v>47.13</v>
+      </c>
+      <c r="I4" s="26">
+        <v>46.45</v>
+      </c>
+      <c r="J4" s="27"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" cm="1">
         <f t="array" ref="A5">IF(C5="P",SUMPRODUCT(--(D$3:D$100&gt;D5),--(C$3:C$100="P"))+1,"")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
@@ -5467,24 +5490,30 @@
       <c r="C5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="26">
         <f>E5+F5</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="3"/>
+        <v>93.34</v>
+      </c>
+      <c r="E5" s="26">
+        <f>MAX(G5:L5)</f>
+        <v>47.36</v>
+      </c>
+      <c r="F5" s="26">
+        <f>IF(COUNT(G5:L5)&gt;1,LARGE(G5:L5,2),0)</f>
+        <v>45.98</v>
+      </c>
+      <c r="G5" s="27">
+        <v>41.93</v>
+      </c>
+      <c r="H5" s="26">
+        <v>45.98</v>
+      </c>
+      <c r="I5" s="26">
+        <v>47.36</v>
+      </c>
+      <c r="J5" s="27"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="28"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="str" cm="1">
@@ -5495,24 +5524,30 @@
         <v>60</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="24">
+      <c r="D6" s="26">
         <f>E6+F6</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="3"/>
+        <v>70.650000000000006</v>
+      </c>
+      <c r="E6" s="26">
+        <f>MAX(G6:L6)</f>
+        <v>44.2</v>
+      </c>
+      <c r="F6" s="26">
+        <f>IF(COUNT(G6:L6)&gt;1,LARGE(G6:L6,2),0)</f>
+        <v>26.45</v>
+      </c>
+      <c r="G6" s="27">
+        <v>44.2</v>
+      </c>
+      <c r="H6" s="26">
+        <v>26.45</v>
+      </c>
+      <c r="I6" s="26">
+        <v>23.1</v>
+      </c>
+      <c r="J6" s="27"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="28"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="str" cm="1">
@@ -5523,24 +5558,28 @@
         <v>61</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="24">
+      <c r="D7" s="26">
         <f>E7+F7</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="3"/>
+        <v>30.75</v>
+      </c>
+      <c r="E7" s="26">
+        <f>MAX(G7:L7)</f>
+        <v>25.75</v>
+      </c>
+      <c r="F7" s="26">
+        <f>IF(COUNT(G7:L7)&gt;1,LARGE(G7:L7,2),0)</f>
+        <v>5</v>
+      </c>
+      <c r="G7" s="27">
+        <v>5</v>
+      </c>
+      <c r="H7" s="26">
+        <v>25.75</v>
+      </c>
+      <c r="I7" s="26"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="28"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="str" cm="1">
@@ -5548,14 +5587,15 @@
         <v/>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="3"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="28"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="str" cm="1">
@@ -5563,14 +5603,15 @@
         <v/>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="3"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="28"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="str" cm="1">
@@ -5578,14 +5619,15 @@
         <v/>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="3"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="28"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="str" cm="1">
@@ -5593,14 +5635,15 @@
         <v/>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="3"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="28"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="str" cm="1">
@@ -5608,14 +5651,15 @@
         <v/>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="3"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="28"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="str" cm="1">
@@ -5623,14 +5667,15 @@
         <v/>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="3"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="28"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="str" cm="1">
@@ -5638,14 +5683,15 @@
         <v/>
       </c>
       <c r="C14" s="9"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="3"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="28"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="str" cm="1">
@@ -5653,14 +5699,15 @@
         <v/>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="3"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="28"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="str" cm="1">
@@ -5668,14 +5715,15 @@
         <v/>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="3"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="28"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="str" cm="1">

</xml_diff>